<commit_message>
Processing speed reliability tests
</commit_message>
<xml_diff>
--- a/basic_data/language_SL_experiments.xlsx
+++ b/basic_data/language_SL_experiments.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
   <si>
     <t>PR_SPEED_YA</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>SEGM_online_VN_DLD_2key_byimg</t>
+  </si>
+  <si>
+    <t>psychometric_analysis_ready</t>
   </si>
 </sst>
 </file>
@@ -25793,7 +25796,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -25803,10 +25806,11 @@
     <col min="2" max="2" width="31.59765625" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.19921875" style="42" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="42" customWidth="1"/>
-    <col min="5" max="16384" width="8.796875" style="42"/>
+    <col min="5" max="5" width="23.3984375" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>82</v>
       </c>
@@ -25819,8 +25823,11 @@
       <c r="D1" s="43" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="str">
         <f>experiments!A2</f>
         <v>background</v>
@@ -25835,8 +25842,11 @@
       <c r="D2" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="str">
         <f>experiments!A3</f>
         <v>background</v>
@@ -25851,8 +25861,11 @@
       <c r="D3" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="str">
         <f>experiments!A4</f>
         <v>background</v>
@@ -25865,10 +25878,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="str">
         <f>experiments!A5</f>
         <v>background</v>
@@ -25881,10 +25897,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="str">
         <f>experiments!A6</f>
         <v>background</v>
@@ -25899,8 +25918,11 @@
       <c r="D6" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="str">
         <f>experiments!A7</f>
         <v>background</v>
@@ -25915,8 +25937,11 @@
       <c r="D7" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="str">
         <f>experiments!A8</f>
         <v>background</v>
@@ -25931,8 +25956,11 @@
       <c r="D8" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="str">
         <f>experiments!A9</f>
         <v>language</v>
@@ -25947,8 +25975,11 @@
       <c r="D9" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="42" t="str">
         <f>experiments!A10</f>
         <v>language</v>
@@ -25963,8 +25994,11 @@
       <c r="D10" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="str">
         <f>experiments!A11</f>
         <v>language</v>
@@ -25979,8 +26013,11 @@
       <c r="D11" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="str">
         <f>experiments!A12</f>
         <v>language</v>
@@ -25995,8 +26032,11 @@
       <c r="D12" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="42" t="str">
         <f>experiments!A13</f>
         <v>language</v>
@@ -26011,8 +26051,11 @@
       <c r="D13" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="42" t="str">
         <f>experiments!A14</f>
         <v>language</v>
@@ -26027,8 +26070,11 @@
       <c r="D14" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="str">
         <f>experiments!A15</f>
         <v>language</v>
@@ -26043,8 +26089,11 @@
       <c r="D15" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="str">
         <f>experiments!A16</f>
         <v>language</v>
@@ -26059,8 +26108,11 @@
       <c r="D16" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="str">
         <f>experiments!A17</f>
         <v>language</v>
@@ -26075,8 +26127,11 @@
       <c r="D17" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="str">
         <f>experiments!A18</f>
         <v>language</v>
@@ -26091,8 +26146,11 @@
       <c r="D18" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="42" t="str">
         <f>experiments!A19</f>
         <v>language</v>
@@ -26107,8 +26165,11 @@
       <c r="D19" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="42" t="str">
         <f>experiments!A20</f>
         <v>SL</v>
@@ -26123,8 +26184,11 @@
       <c r="D20" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="str">
         <f>experiments!A21</f>
         <v>SL</v>
@@ -26139,8 +26203,11 @@
       <c r="D21" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="42" t="str">
         <f>experiments!A22</f>
         <v>SL</v>
@@ -26155,8 +26222,11 @@
       <c r="D22" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="42" t="str">
         <f>experiments!A23</f>
         <v>SL</v>
@@ -26171,8 +26241,11 @@
       <c r="D23" s="42" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="42" t="str">
         <f>experiments!A24</f>
         <v>SL</v>
@@ -26187,8 +26260,11 @@
       <c r="D24" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="str">
         <f>experiments!A25</f>
         <v>SL</v>
@@ -26203,8 +26279,11 @@
       <c r="D25" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="42" t="str">
         <f>experiments!A26</f>
         <v>SL</v>
@@ -26219,8 +26298,11 @@
       <c r="D26" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="42" t="str">
         <f>experiments!A27</f>
         <v>SL</v>
@@ -26235,8 +26317,11 @@
       <c r="D27" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="42" t="str">
         <f>experiments!A28</f>
         <v>SL</v>
@@ -26251,8 +26336,11 @@
       <c r="D28" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="42" t="str">
         <f>experiments!A29</f>
         <v>SL</v>
@@ -26267,8 +26355,11 @@
       <c r="D29" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="str">
         <f>experiments!A30</f>
         <v>TOM</v>
@@ -26283,8 +26374,11 @@
       <c r="D30" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="42" t="str">
         <f>experiments!A31</f>
         <v>TOM</v>
@@ -26299,8 +26393,11 @@
       <c r="D31" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="42" t="str">
         <f>experiments!A32</f>
         <v>BLP</v>
@@ -26315,8 +26412,11 @@
       <c r="D32" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="42" t="str">
         <f>experiments!A33</f>
         <v>BLP</v>
@@ -26331,8 +26431,11 @@
       <c r="D33" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="42" t="str">
         <f>experiments!A34</f>
         <v>BLP</v>
@@ -26347,8 +26450,11 @@
       <c r="D34" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="42" t="str">
         <f>experiments!A35</f>
         <v>BLP</v>
@@ -26363,8 +26469,11 @@
       <c r="D35" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="42" t="str">
         <f>experiments!A36</f>
         <v>demography</v>
@@ -26379,8 +26488,11 @@
       <c r="D36" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="42" t="str">
         <f>experiments!A37</f>
         <v>demography</v>
@@ -26395,8 +26507,11 @@
       <c r="D37" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="42" t="str">
         <f>experiments!A38</f>
         <v>demography</v>
@@ -26411,8 +26526,11 @@
       <c r="D38" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="42" t="str">
         <f>experiments!A39</f>
         <v>demography</v>
@@ -26427,8 +26545,11 @@
       <c r="D39" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="42" t="str">
         <f>experiments!A40</f>
         <v>demography</v>
@@ -26443,8 +26564,11 @@
       <c r="D40" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="42" t="str">
         <f>experiments!A41</f>
         <v>demography</v>
@@ -26459,8 +26583,11 @@
       <c r="D41" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="42" t="str">
         <f>experiments!A42</f>
         <v>demography</v>
@@ -26475,8 +26602,11 @@
       <c r="D42" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="42" t="str">
         <f>experiments!A43</f>
         <v>demography</v>
@@ -26491,8 +26621,11 @@
       <c r="D43" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="42">
         <f>experiments!A45</f>
         <v>0</v>
@@ -26502,7 +26635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="42">
         <f>experiments!A46</f>
         <v>0</v>
@@ -26512,7 +26645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="42">
         <f>experiments!A47</f>
         <v>0</v>
@@ -26522,7 +26655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="42">
         <f>experiments!A48</f>
         <v>0</v>
@@ -26534,7 +26667,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D47">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -26546,7 +26679,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C47">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -26558,6 +26691,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D47">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E47">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
self paced reading data calculated
</commit_message>
<xml_diff>
--- a/basic_data/language_SL_experiments.xlsx
+++ b/basic_data/language_SL_experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="2" r:id="rId1"/>
@@ -25790,7 +25790,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
rec_vocab SAT SL data updated
</commit_message>
<xml_diff>
--- a/basic_data/language_SL_experiments.xlsx
+++ b/basic_data/language_SL_experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="125">
   <si>
     <t>PR_SPEED_YA</t>
   </si>
@@ -25836,14 +25836,14 @@
         <f>experiments!B2</f>
         <v>DigitSpan</v>
       </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0</v>
+      <c r="C2" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -25856,7 +25856,7 @@
         <v>n_back</v>
       </c>
       <c r="C3" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="42">
         <v>0</v>
@@ -25913,7 +25913,7 @@
         <v>simon</v>
       </c>
       <c r="C6" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="42">
         <v>0</v>
@@ -25932,7 +25932,7 @@
         <v>stroop</v>
       </c>
       <c r="C7" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="42">
         <v>0</v>
@@ -25950,14 +25950,14 @@
         <f>experiments!B8</f>
         <v>Raven</v>
       </c>
-      <c r="C8" s="42">
-        <v>0</v>
-      </c>
-      <c r="D8" s="42">
-        <v>0</v>
-      </c>
-      <c r="E8" s="42">
-        <v>0</v>
+      <c r="C8" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -25970,10 +25970,10 @@
         <v>adult_trog</v>
       </c>
       <c r="C9" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="42">
         <v>0</v>
@@ -26046,10 +26046,10 @@
         <v>menyet</v>
       </c>
       <c r="C13" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="42">
         <v>0</v>
@@ -26064,14 +26064,14 @@
         <f>experiments!B14</f>
         <v>OMR</v>
       </c>
-      <c r="C14" s="42">
-        <v>0</v>
-      </c>
-      <c r="D14" s="42">
-        <v>0</v>
-      </c>
-      <c r="E14" s="42">
-        <v>0</v>
+      <c r="C14" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -26122,10 +26122,10 @@
         <v>Self_paced_reading</v>
       </c>
       <c r="C17" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="42">
         <v>0</v>
@@ -26141,10 +26141,10 @@
         <v>trog_javitott</v>
       </c>
       <c r="C18" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="42">
         <v>0</v>
@@ -26159,14 +26159,14 @@
         <f>experiments!B19</f>
         <v>KOBAK</v>
       </c>
-      <c r="C19" s="42">
-        <v>0</v>
-      </c>
-      <c r="D19" s="42">
-        <v>0</v>
-      </c>
-      <c r="E19" s="42">
-        <v>0</v>
+      <c r="C19" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>